<commit_message>
modified format, cleaner presentation
</commit_message>
<xml_diff>
--- a/Results_comparison_reviewed_v3.xlsx
+++ b/Results_comparison_reviewed_v3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erivero/Documents/MBD_IE/t2/Forecasting_times_series/homework1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erivero/Documents/MBD_IE/t2/Forecasting_times_series/homework1/inGit/TimeSeriesAnalysis_HM1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E820A5-B5DB-664E-A352-772A4CF5B6F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FEC9A6-60E5-AD4C-8F48-E40EBC217409}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23980" yWindow="1280" windowWidth="19160" windowHeight="17500" xr2:uid="{0F7D505D-79A6-1D45-A89E-88ABC1A21B45}"/>
+    <workbookView xWindow="20" yWindow="520" windowWidth="17040" windowHeight="21060" xr2:uid="{0F7D505D-79A6-1D45-A89E-88ABC1A21B45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -156,10 +156,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -462,7 +458,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>